<commit_message>
save 05/02 / Création de piece model
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="101">
   <si>
     <t xml:space="preserve">Objet : </t>
   </si>
@@ -309,6 +309,24 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>convertDH</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>Converti le décimal en hexa</t>
+  </si>
+  <si>
+    <t>convertHD</t>
+  </si>
+  <si>
+    <t>hexa</t>
+  </si>
+  <si>
+    <t>Converti le hexa en decimal</t>
   </si>
 </sst>
 </file>
@@ -677,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,9 +1007,15 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="O9" s="6"/>
@@ -1018,6 +1042,18 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6" t="s">
         <v>74</v>
@@ -1044,14 +1080,12 @@
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6" t="s">
         <v>76</v>
@@ -1072,16 +1106,6 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="H12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -1096,18 +1120,12 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="H13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
@@ -1126,16 +1144,14 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="I14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="O14" s="7"/>
@@ -1154,15 +1170,17 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="I15" s="2" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1180,13 +1198,13 @@
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1215,9 +1233,15 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="O17" s="7"/>
@@ -1244,17 +1268,15 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="H18" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1310,6 +1332,20 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
+      <c r="H20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
       <c r="O20" s="7" t="s">
         <v>2</v>
       </c>
@@ -1338,14 +1374,12 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7" t="s">
         <v>83</v>
@@ -1372,16 +1406,6 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="H22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
@@ -1402,18 +1426,12 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="H23" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="H23" s="5"/>
       <c r="I23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
@@ -1430,16 +1448,14 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="I24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
@@ -1456,15 +1472,17 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="I25" s="5" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
@@ -1484,13 +1502,13 @@
       <c r="F26" s="1"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
@@ -1508,18 +1526,18 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -1534,16 +1552,18 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
@@ -1556,12 +1576,18 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -1574,6 +1600,16 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -1582,6 +1618,12 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">

</xml_diff>